<commit_message>
fixed a typo for WR1
</commit_message>
<xml_diff>
--- a/data/derived_data/proposed_iptds_sites_20240411.xlsx
+++ b/data/derived_data/proposed_iptds_sites_20240411.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B549DD9-7E70-420F-89AD-4057410ADF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5672E73D-78AE-4596-A5A5-ED3B97ED0832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="135">
   <si>
     <t>site_code</t>
   </si>
@@ -433,9 +433,6 @@
   </si>
   <si>
     <t>Upgrade to IS1001 MC to span river and increase read range</t>
-  </si>
-  <si>
-    <t>Upgrade to IS1001 MC to spawn river and increase read range</t>
   </si>
   <si>
     <t>HIGH</t>
@@ -785,7 +782,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E54"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -865,7 +862,7 @@
         <v>-114.0744</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>127</v>
@@ -885,7 +882,7 @@
         <v>-114.35290000000001</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>119</v>
@@ -905,7 +902,7 @@
         <v>-114.30289999999999</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1107,7 +1104,7 @@
         <v>-114.9449</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1224,7 +1221,7 @@
         <v>-116.3293</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>120</v>
@@ -1244,7 +1241,7 @@
         <v>-116.306603</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1261,7 +1258,7 @@
         <v>-116.2645</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1345,7 +1342,7 @@
         <v>128</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1362,10 +1359,10 @@
         <v>-115.97776</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1615,7 +1612,7 @@
         <v>128</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1635,7 +1632,7 @@
         <v>128</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1740,7 +1737,7 @@
         <v>128</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushed updates to leaflet
</commit_message>
<xml_diff>
--- a/data/derived_data/proposed_iptds_sites_20240411.xlsx
+++ b/data/derived_data/proposed_iptds_sites_20240411.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5672E73D-78AE-4596-A5A5-ED3B97ED0832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7B4F43-6DAA-445C-B33D-0E3E5EDECF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="141">
   <si>
     <t>site_code</t>
   </si>
@@ -399,52 +399,70 @@
     <t>LOW</t>
   </si>
   <si>
-    <t>Alternative Locations: East Fork Salmon</t>
-  </si>
-  <si>
-    <t>Alternative Locations: Slate Creek, Whitebird Creek</t>
-  </si>
-  <si>
     <t>USU (Proposed)</t>
   </si>
   <si>
     <t>USI (Proposed)</t>
   </si>
   <si>
-    <t>Upgrade upstream and/or downstream array(s) to FS1001 MUX</t>
-  </si>
-  <si>
-    <t>Planned upsgrade to IS1001 MC</t>
-  </si>
-  <si>
-    <t>Consider decommissioning if LC1 can be converted to a two-pass configuration; alternatively, consider moving upstream to below core spawning areas</t>
-  </si>
-  <si>
-    <t>Consider upgrade to IS1001 MC if sufficient distance btw arrays can be achieved</t>
-  </si>
-  <si>
-    <t>Ideally, located below Morgan Creek and above population boundary. Locations near Challis, ID could also be considered</t>
-  </si>
-  <si>
     <t>MED</t>
   </si>
   <si>
-    <t>Upgrade to IS1001 MC to increase read range</t>
-  </si>
-  <si>
-    <t>Upgrade to IS1001 MC to span river and increase read range</t>
-  </si>
-  <si>
     <t>HIGH</t>
   </si>
   <si>
-    <t>Proposed site not necessary if weir is operated annually and is reliable</t>
-  </si>
-  <si>
-    <t>If not already, consider upgrade to IS1001 to increase read range</t>
-  </si>
-  <si>
-    <t>Move to lower boundary of CRSFC-s population</t>
+    <t>Ideally, located below Morgan Creek and above population boundary. Locations near Challis, ID could also be considered.</t>
+  </si>
+  <si>
+    <t>Upgrade to IS1001 MC to span river and increase read range.</t>
+  </si>
+  <si>
+    <t>Upgrade upstream and/or downstream array(s) to FS1001 MUX.</t>
+  </si>
+  <si>
+    <t>If not already, consider upgrade to IS1001 to increase read range.</t>
+  </si>
+  <si>
+    <t>Move to lower boundary of CRSFC-s population.</t>
+  </si>
+  <si>
+    <t>Consider decommissioning if LC1 can be converted to a two-pass configuration; alternatively, consider moving upstream to below core spawning areas.</t>
+  </si>
+  <si>
+    <t>Upgrade to IS1001 MC to increase read range.</t>
+  </si>
+  <si>
+    <t>Proposed site not necessary if weir is operated annually and is reliable.</t>
+  </si>
+  <si>
+    <t>If transfer to IPTDS O&amp;M project is not desired, ensure long-term funding.</t>
+  </si>
+  <si>
+    <t>Alternative locations: East Fork Salmon River.</t>
+  </si>
+  <si>
+    <t>Move upstream to proposed USI location.</t>
+  </si>
+  <si>
+    <t>Planned upsgrade to IS1001 MC. Alternatively, LLR could be considered for upgrade to IS1001 MC to increase juvenile detections.</t>
+  </si>
+  <si>
+    <t>Alternate locations: upper Chamberlain, Sabe, Bargamin, Warren, Crooked, or Sheep creeks.</t>
+  </si>
+  <si>
+    <t>Alternative locations: Slate Creek, Whitebird Creek.</t>
+  </si>
+  <si>
+    <t>Consider funding either SC3 or SC4 to provide detections to estimate abundance at SC2 at proposed new location.</t>
+  </si>
+  <si>
+    <t>Consider upgrade to IS1001 MC and tandem arrays if sufficient distance btw arrays can be achieved.</t>
+  </si>
+  <si>
+    <t>One of LAP, JUL, or LAW should be funded to provide monitoring in the CRLMA-s population. LAP or JUL would be preferred to continue time-series of estimates.</t>
+  </si>
+  <si>
+    <t>New site could be a single-pass array.</t>
   </si>
 </sst>
 </file>
@@ -782,7 +800,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -847,99 +865,105 @@
       <c r="E3" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3">
-        <v>44.677300000000002</v>
+        <v>44.253700000000002</v>
       </c>
       <c r="D4" s="3">
-        <v>-114.0744</v>
+        <v>-114.35290000000001</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3">
-        <v>44.253700000000002</v>
+        <v>44.245899999999999</v>
       </c>
       <c r="D5" s="3">
-        <v>-114.35290000000001</v>
+        <v>-114.30289999999999</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>44.245899999999999</v>
+        <v>44.677300000000002</v>
       </c>
       <c r="D6" s="3">
-        <v>-114.30289999999999</v>
+        <v>-114.0744</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3">
-        <v>45.028530000000003</v>
+        <v>44.889763000000002</v>
       </c>
       <c r="D7" s="3">
-        <v>-113.916319</v>
+        <v>-113.964145</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3">
-        <v>44.889763000000002</v>
+        <v>45.028530000000003</v>
       </c>
       <c r="D8" s="3">
-        <v>-113.964145</v>
+        <v>-113.916319</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1002,9 +1026,11 @@
       <c r="D12" s="3">
         <v>-113.62472099999999</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1089,6 +1115,9 @@
       <c r="E17" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="F17" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -1104,7 +1133,10 @@
         <v>-114.9449</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1181,10 +1213,10 @@
         <v>-115.53315000000001</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1201,10 +1233,10 @@
         <v>-115.73302</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1221,10 +1253,10 @@
         <v>-116.3293</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1241,7 +1273,7 @@
         <v>-116.306603</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1258,7 +1290,7 @@
         <v>-116.2645</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1275,7 +1307,7 @@
         <v>-115.56588600000001</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1292,7 +1324,7 @@
         <v>-115.515533</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1339,10 +1371,10 @@
         <v>-115.981313</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1359,10 +1391,10 @@
         <v>-115.97776</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1379,7 +1411,10 @@
         <v>-115.815972</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1396,7 +1431,10 @@
         <v>-115.6341</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1430,10 +1468,10 @@
         <v>-115.97615999999999</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1450,10 +1488,10 @@
         <v>-115.933747</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1470,7 +1508,10 @@
         <v>-116.812535</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1487,7 +1528,10 @@
         <v>-116.709318</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1504,7 +1548,10 @@
         <v>-116.02898500000001</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1521,7 +1568,7 @@
         <v>-116.750231</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>129</v>
@@ -1609,10 +1656,10 @@
         <v>-117.903379</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1629,10 +1676,10 @@
         <v>-117.733757</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1651,6 +1698,9 @@
       <c r="E49" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="F49" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
@@ -1668,6 +1718,9 @@
       <c r="E50" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="F50" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
@@ -1683,7 +1736,10 @@
         <v>-117.45412399999999</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1734,10 +1790,10 @@
         <v>-117.22450000000001</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incorporated comments from rk
</commit_message>
<xml_diff>
--- a/data/derived_data/proposed_iptds_sites_20240411.xlsx
+++ b/data/derived_data/proposed_iptds_sites_20240411.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7B4F43-6DAA-445C-B33D-0E3E5EDECF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23477C72-AB66-4ABB-87C4-967EE3A8549B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="143">
   <si>
     <t>site_code</t>
   </si>
@@ -444,9 +444,6 @@
     <t>Move upstream to proposed USI location.</t>
   </si>
   <si>
-    <t>Planned upsgrade to IS1001 MC. Alternatively, LLR could be considered for upgrade to IS1001 MC to increase juvenile detections.</t>
-  </si>
-  <si>
     <t>Alternate locations: upper Chamberlain, Sabe, Bargamin, Warren, Crooked, or Sheep creeks.</t>
   </si>
   <si>
@@ -463,13 +460,22 @@
   </si>
   <si>
     <t>New site could be a single-pass array.</t>
+  </si>
+  <si>
+    <t>Either LLR or both HYC and LRW could long-term be considered for consolidation to single-pass arrays, especially if sites(s) were upgraded with IS1001 MC(s).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planned upgrade to IS1001 MC. Alternatively, LLR could be considered for upgrade to IS1001 MC to increase juvenile detections. Either LLR or both HYC and LRW could long-term be considered for consolidation to single-pass arrays, especially if sites(s) were upgraded with IS1001 MC(s).   </t>
+  </si>
+  <si>
+    <t>If feasible, SW2 could be moved to the end of the Selway Road which would allow parsing of the SEMOO and SEUMA populations from SEMEA.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,6 +486,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -505,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -517,6 +530,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,7 +814,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -980,6 +994,9 @@
         <v>-113.885278</v>
       </c>
       <c r="E9" s="4"/>
+      <c r="F9" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1012,6 +1029,9 @@
         <v>-113.63193699999999</v>
       </c>
       <c r="E11" s="4"/>
+      <c r="F11" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1030,7 +1050,7 @@
         <v>121</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1136,7 +1156,7 @@
         <v>122</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1256,7 +1276,7 @@
         <v>122</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1326,6 +1346,9 @@
       <c r="E29" s="4" t="s">
         <v>122</v>
       </c>
+      <c r="F29" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -1414,7 +1437,7 @@
         <v>121</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1434,7 +1457,7 @@
         <v>121</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1471,7 +1494,7 @@
         <v>121</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1511,7 +1534,7 @@
         <v>121</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1531,7 +1554,7 @@
         <v>121</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1551,7 +1574,7 @@
         <v>121</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1699,7 +1722,7 @@
         <v>118</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>